<commit_message>
Fortsatte med excel relationsdatabasen
</commit_message>
<xml_diff>
--- a/slutprojekt/excel_mys/Databaser och hemliga lådor.xlsx
+++ b/slutprojekt/excel_mys/Databaser och hemliga lådor.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
   <si>
     <t>Field</t>
   </si>
@@ -36,6 +36,57 @@
   </si>
   <si>
     <t>Users</t>
+  </si>
+  <si>
+    <t>PRI</t>
+  </si>
+  <si>
+    <t>int(6)</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>First_Name</t>
+  </si>
+  <si>
+    <t>varchar(32)</t>
+  </si>
+  <si>
+    <t>Last_Name</t>
+  </si>
+  <si>
+    <t>Mail</t>
+  </si>
+  <si>
+    <t>Personal_Number</t>
+  </si>
+  <si>
+    <t>UNI</t>
+  </si>
+  <si>
+    <t>Adress</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Postal_Code</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Passwords</t>
+  </si>
+  <si>
+    <t>MUL</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Purchases</t>
   </si>
 </sst>
 </file>
@@ -77,7 +128,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -86,33 +137,61 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -123,27 +202,81 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -425,121 +558,230 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="J14" sqref="J14:J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="17.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="5" max="6" width="12.5703125" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="E1" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="17"/>
+      <c r="G1" s="18"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
-      <c r="B13" s="3"/>
+      <c r="B13" s="2"/>
       <c r="C13" s="2"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="2"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="2"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="2"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="6"/>
+      <c r="C14" s="7"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="11"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="2"/>
+      <c r="A17" s="10"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="12"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="5"/>
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="E1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Vidare uppgraderingar på excel
</commit_message>
<xml_diff>
--- a/slutprojekt/excel_mys/Databaser och hemliga lådor.xlsx
+++ b/slutprojekt/excel_mys/Databaser och hemliga lådor.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="48">
   <si>
     <t>Field</t>
   </si>
@@ -86,7 +86,88 @@
     <t>Password</t>
   </si>
   <si>
-    <t>Purchases</t>
+    <t>Products</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>bigint(10)</t>
+  </si>
+  <si>
+    <t>Disease</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>int(10)</t>
+  </si>
+  <si>
+    <t>Product_Name</t>
+  </si>
+  <si>
+    <t>Categories</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>varchar(64)</t>
+  </si>
+  <si>
+    <t>text(100)</t>
+  </si>
+  <si>
+    <t>Orders</t>
+  </si>
+  <si>
+    <t>bigint(12)</t>
+  </si>
+  <si>
+    <t>Order_Date</t>
+  </si>
+  <si>
+    <t>Extra</t>
+  </si>
+  <si>
+    <t>int(8)</t>
+  </si>
+  <si>
+    <t>timestamp</t>
+  </si>
+  <si>
+    <t>float(8)</t>
+  </si>
+  <si>
+    <t>text(500)</t>
+  </si>
+  <si>
+    <t>Communicator</t>
+  </si>
+  <si>
+    <t>Order_Details</t>
+  </si>
+  <si>
+    <t>Customer_Number</t>
+  </si>
+  <si>
+    <t>Order_Number</t>
+  </si>
+  <si>
+    <t>Product_Number</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Creation_Date</t>
+  </si>
+  <si>
+    <t>Expiration_Date</t>
+  </si>
+  <si>
+    <t>Weight</t>
   </si>
 </sst>
 </file>
@@ -102,7 +183,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -127,8 +208,38 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -232,15 +343,25 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -248,12 +369,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -266,9 +381,22 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -277,6 +405,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -558,10 +695,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14:J15"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -569,217 +706,448 @@
     <col min="1" max="1" width="17.140625" customWidth="1"/>
     <col min="2" max="2" width="14.85546875" customWidth="1"/>
     <col min="3" max="3" width="15.42578125" customWidth="1"/>
-    <col min="5" max="6" width="12.5703125" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" customWidth="1"/>
     <col min="7" max="7" width="13.42578125" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="E1" s="16" t="s">
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="E1" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="17"/>
-      <c r="G1" s="18"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="F1" s="23"/>
+      <c r="G1" s="24"/>
+      <c r="I1" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" s="23"/>
+      <c r="K1" s="24"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="E2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="F2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="E3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="3"/>
+      <c r="I3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" s="16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="B4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="E4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="3"/>
+      <c r="I4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="B5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="E5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="3"/>
+      <c r="I5" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K5" s="20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="B6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="E6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="3"/>
+      <c r="I6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K6" s="3"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="5" t="s">
+      <c r="B7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="E7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="3"/>
+      <c r="I7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K7" s="3"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="B8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="E8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="3"/>
+      <c r="I8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K8" s="3"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="B9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="E9" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K9" s="3"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="B10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="I10" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="K10" s="3"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+      <c r="B11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="E11" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11" s="23"/>
+      <c r="G11" s="24"/>
+      <c r="I11" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="K11" s="3"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="E12" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="E13" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G13" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="7"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
+      <c r="B14" s="26"/>
+      <c r="C14" s="27"/>
+      <c r="E14" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
+      <c r="E15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" s="11"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="10"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="12"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
+      <c r="B16" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="8"/>
+      <c r="E16" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G16" s="3"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="E19" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="F19" s="23"/>
+      <c r="G19" s="24"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E20" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="G20" s="21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E21" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G21" s="20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E22" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G22" s="3"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E23" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="6">
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="E19:G19"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A14:C14"/>
     <mergeCell ref="E1:G1"/>
+    <mergeCell ref="E11:G11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Databaserna för slutprojektet klara
</commit_message>
<xml_diff>
--- a/slutprojekt/excel_mys/Databaser och hemliga lådor.xlsx
+++ b/slutprojekt/excel_mys/Databaser och hemliga lådor.xlsx
@@ -167,7 +167,7 @@
     <t>Weight</t>
   </si>
   <si>
-    <t>Communtication</t>
+    <t>Communticater</t>
   </si>
 </sst>
 </file>
@@ -698,7 +698,7 @@
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Flyttade om några filer, gjorde om css så det ser behagligt ut vid mobil vy, satte in en tragisk for loop som skriver ut meddelande + break line även relationsdatabas uppdaterad
</commit_message>
<xml_diff>
--- a/slutprojekt/excel_mys/Databaser och hemliga lådor.xlsx
+++ b/slutprojekt/excel_mys/Databaser och hemliga lådor.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="66">
   <si>
     <t>Field</t>
   </si>
@@ -35,9 +35,6 @@
     <t>Key</t>
   </si>
   <si>
-    <t>Users</t>
-  </si>
-  <si>
     <t>PRI</t>
   </si>
   <si>
@@ -86,9 +83,6 @@
     <t>Password</t>
   </si>
   <si>
-    <t>Products</t>
-  </si>
-  <si>
     <t>Price</t>
   </si>
   <si>
@@ -167,7 +161,67 @@
     <t>Weight</t>
   </si>
   <si>
-    <t>Communticater</t>
+    <t>Ticket</t>
+  </si>
+  <si>
+    <t>departments</t>
+  </si>
+  <si>
+    <t>reply</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>int(11)</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>auto_inc</t>
+  </si>
+  <si>
+    <t>Communicator</t>
+  </si>
+  <si>
+    <t>products_list</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>product_name</t>
+  </si>
+  <si>
+    <t>produt_desc</t>
+  </si>
+  <si>
+    <t>product_code</t>
+  </si>
+  <si>
+    <t>product_image</t>
+  </si>
+  <si>
+    <t>product_price</t>
+  </si>
+  <si>
+    <t>varchar(60)</t>
+  </si>
+  <si>
+    <t>decimal(10,2</t>
+  </si>
+  <si>
+    <t>products</t>
+  </si>
+  <si>
+    <t>users</t>
+  </si>
+  <si>
+    <t>Databas namn = st</t>
   </si>
 </sst>
 </file>
@@ -183,7 +237,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -238,6 +292,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -360,7 +426,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -415,6 +481,26 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -695,10 +781,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -715,17 +801,17 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
-        <v>3</v>
+        <v>64</v>
       </c>
       <c r="B1" s="25"/>
       <c r="C1" s="25"/>
       <c r="E1" s="22" t="s">
-        <v>20</v>
+        <v>63</v>
       </c>
       <c r="F1" s="23"/>
       <c r="G1" s="24"/>
       <c r="I1" s="22" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="J1" s="23"/>
       <c r="K1" s="24"/>
@@ -741,13 +827,13 @@
         <v>2</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I2" s="13" t="s">
         <v>0</v>
@@ -761,158 +847,158 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G3" s="3"/>
       <c r="I3" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="K3" s="16" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>8</v>
       </c>
       <c r="C4" s="3"/>
       <c r="E4" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G4" s="3"/>
       <c r="I4" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="K4" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" s="3"/>
       <c r="E5" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G5" s="3"/>
       <c r="I5" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="K5" s="20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" s="3"/>
       <c r="E6" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G6" s="3"/>
       <c r="I6" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K6" s="3"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>12</v>
-      </c>
       <c r="E7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="G7" s="3"/>
       <c r="I7" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K7" s="3"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" s="3"/>
       <c r="E8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>30</v>
       </c>
       <c r="G8" s="3"/>
       <c r="I8" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K8" s="3"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9" s="3"/>
       <c r="E9" s="9" t="s">
@@ -925,50 +1011,50 @@
         <v>2</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="K9" s="3"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C10" s="3"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="I10" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="K10" s="3"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C11" s="3"/>
       <c r="E11" s="22" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
       <c r="I11" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="K11" s="3"/>
     </row>
@@ -977,13 +1063,13 @@
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="E12" s="14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
@@ -994,13 +1080,13 @@
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="E13" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G13" s="20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
@@ -1008,15 +1094,15 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14" s="26"/>
       <c r="C14" s="27"/>
       <c r="E14" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G14" s="3"/>
       <c r="I14" s="3"/>
@@ -1025,19 +1111,19 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G15" s="3"/>
       <c r="I15" s="3"/>
@@ -1046,24 +1132,24 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C16" s="8"/>
       <c r="E16" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G16" s="3"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>0</v>
       </c>
@@ -1083,53 +1169,119 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" s="32"/>
+      <c r="C19" s="33"/>
       <c r="E19" s="22" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F19" s="23"/>
       <c r="G19" s="24"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I19" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="J19" s="29"/>
+      <c r="K19" s="29"/>
+      <c r="L19" s="34"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>3</v>
+      </c>
       <c r="E20" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="G20" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="I20" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="J20" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="K20" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="L20" s="28" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21" s="28"/>
+      <c r="E21" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G21" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="I21" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="J21" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="K21" s="28"/>
+      <c r="L21" s="28"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22" s="28"/>
+      <c r="E22" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F20" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="G20" s="21" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E21" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G21" s="20" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E22" s="3" t="s">
-        <v>43</v>
-      </c>
       <c r="F22" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G22" s="3"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I22" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="J22" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="K22" s="28"/>
+      <c r="L22" s="28"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" s="28"/>
       <c r="E23" s="9" t="s">
         <v>0</v>
       </c>
@@ -1139,15 +1291,77 @@
       <c r="G23" s="9" t="s">
         <v>2</v>
       </c>
+      <c r="I23" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="J23" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="K23" s="28"/>
+      <c r="L23" s="28"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="B24" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="C24" s="28"/>
+      <c r="I24" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="J24" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="K24" s="28"/>
+      <c r="L24" s="28"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="B25" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="C25" s="28"/>
+      <c r="E25" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="I25" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="J25" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="K25" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="L25" s="28" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" s="28" t="s">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="8">
     <mergeCell ref="I1:K1"/>
     <mergeCell ref="E19:G19"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A14:C14"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="E11:G11"/>
+    <mergeCell ref="I19:L19"/>
+    <mergeCell ref="A19:C19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>